<commit_message>
Added Testing on Floors
</commit_message>
<xml_diff>
--- a/Seneca_Phase3/unit_testing/database.xlsx
+++ b/Seneca_Phase3/unit_testing/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRAFT-pytorch\unit_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\floorplan\Seneca_Phase3\unit_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,66 @@
   </si>
   <si>
     <t>Bathrooms</t>
+  </si>
+  <si>
+    <t>Floors</t>
+  </si>
+  <si>
+    <t>Ground Floor</t>
+  </si>
+  <si>
+    <t>8-26</t>
+  </si>
+  <si>
+    <t>9-26</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3-11</t>
+  </si>
+  <si>
+    <t>9-23</t>
+  </si>
+  <si>
+    <t>14-22</t>
+  </si>
+  <si>
+    <t>2-11</t>
+  </si>
+  <si>
+    <t>3-7</t>
+  </si>
+  <si>
+    <t>4-28</t>
+  </si>
+  <si>
+    <t>13-23</t>
+  </si>
+  <si>
+    <t>3-23</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10-28</t>
+  </si>
+  <si>
+    <t>24-28</t>
+  </si>
+  <si>
+    <t>25-27</t>
+  </si>
+  <si>
+    <t>4-9</t>
+  </si>
+  <si>
+    <t>9-32</t>
   </si>
 </sst>
 </file>
@@ -166,13 +226,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -183,6 +251,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:G25" totalsRowShown="0">
+  <autoFilter ref="A1:G25"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Inner"/>
+    <tableColumn id="3" name="Outer"/>
+    <tableColumn id="4" name="Dens"/>
+    <tableColumn id="5" name="Bedrooms"/>
+    <tableColumn id="6" name="Bathrooms">
+      <calculatedColumnFormula>1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Floors" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,19 +588,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" customWidth="1"/>
+    <col min="7" max="7" width="22.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +621,11 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -558,8 +649,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -583,8 +677,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -608,8 +705,11 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -631,8 +731,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -656,8 +759,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -681,8 +787,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -706,8 +815,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -731,8 +843,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -756,8 +871,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -781,8 +899,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -806,8 +927,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -831,8 +955,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -856,8 +983,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -881,8 +1011,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -906,8 +1039,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -931,8 +1067,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -956,8 +1095,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -981,8 +1123,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1006,8 +1151,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1031,8 +1179,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1056,8 +1207,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1081,8 +1235,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1106,8 +1263,11 @@
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1131,9 +1291,15 @@
         <f>1</f>
         <v>1</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated unit testing on floor number
</commit_message>
<xml_diff>
--- a/Seneca_Phase3/unit_testing/database.xlsx
+++ b/Seneca_Phase3/unit_testing/database.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -145,46 +145,49 @@
     <t>2</t>
   </si>
   <si>
-    <t>3-11</t>
-  </si>
-  <si>
-    <t>9-23</t>
-  </si>
-  <si>
-    <t>14-22</t>
-  </si>
-  <si>
-    <t>2-11</t>
-  </si>
-  <si>
     <t>3-7</t>
   </si>
   <si>
-    <t>4-28</t>
-  </si>
-  <si>
-    <t>13-23</t>
-  </si>
-  <si>
-    <t>3-23</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
-    <t>10-28</t>
-  </si>
-  <si>
-    <t>24-28</t>
-  </si>
-  <si>
-    <t>25-27</t>
-  </si>
-  <si>
     <t>4-9</t>
   </si>
   <si>
     <t>9-32</t>
+  </si>
+  <si>
+    <t>9-11,8,3-7</t>
+  </si>
+  <si>
+    <t>9,11,13,15,17,19,21,23</t>
+  </si>
+  <si>
+    <t>14,16,18,20,22</t>
+  </si>
+  <si>
+    <t>2,3,6,7,10,11</t>
+  </si>
+  <si>
+    <t>4,6,8,10,12,14,16,18,20,22,24,26,28</t>
+  </si>
+  <si>
+    <t>13,15,17,19,21,23</t>
+  </si>
+  <si>
+    <t>3,5,7,9,11,13,15,17,19,21,23</t>
+  </si>
+  <si>
+    <t>10,12,14,16,18,20,22,24,26,28</t>
+  </si>
+  <si>
+    <t>2,3-7,8,9-11</t>
+  </si>
+  <si>
+    <t>24,26,28</t>
+  </si>
+  <si>
+    <t>25,27</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -650,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -678,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -928,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -956,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -984,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1012,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1040,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1068,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1096,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1124,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1152,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1180,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1208,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1236,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1264,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1292,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>